<commit_message>
tried mediapipe in test2.py and test3.py
Finding it hard to detect the face when low res or if far from camera
</commit_message>
<xml_diff>
--- a/Data/Gender Detection/Stats.xlsx
+++ b/Data/Gender Detection/Stats.xlsx
@@ -31,7 +31,7 @@
     <t>Non-Human Screen Time</t>
   </si>
   <si>
-    <t>Local 10 News Brief 032622 Evening Edition240p</t>
+    <t>Australia news anchors caught in Djokovic hot mic360p</t>
   </si>
 </sst>
 </file>
@@ -417,16 +417,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>104.3042</v>
+        <v>62.06666666666667</v>
       </c>
       <c r="C2">
-        <v>19.9199</v>
+        <v>10.1</v>
       </c>
       <c r="D2">
-        <v>21.85516666666667</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="E2">
-        <v>57.42403333333333</v>
+        <v>10.16666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Face Detection using RetinaFace
</commit_message>
<xml_diff>
--- a/Data/Gender Detection/Stats.xlsx
+++ b/Data/Gender Detection/Stats.xlsx
@@ -31,7 +31,7 @@
     <t>Non-Human Screen Time</t>
   </si>
   <si>
-    <t>Australia news anchors caught in Djokovic hot mic360p</t>
+    <t>Local 10 News Brief 032622 Evening Edition720p</t>
   </si>
 </sst>
 </file>
@@ -417,16 +417,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>62.06666666666667</v>
+        <v>104.3042</v>
       </c>
       <c r="C2">
-        <v>10.1</v>
+        <v>0.1334666666666667</v>
       </c>
       <c r="D2">
-        <v>0.9666666666666667</v>
+        <v>4.270933333333334</v>
       </c>
       <c r="E2">
-        <v>10.16666666666667</v>
+        <v>10.54386666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>